<commit_message>
Change One Rev 1
</commit_message>
<xml_diff>
--- a/Test Results.xlsx
+++ b/Test Results.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://smartbear-my.sharepoint.com/personal/jonathan_fortunati_smartbear_com/Documents/Projects/documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Melvin.Gage\Desktop\DocumentReview\Changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF87FB04-D32C-4BA0-97AE-7C0FBCF5305A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9108"/>
+    <workbookView xWindow="40680" yWindow="2280" windowWidth="21600" windowHeight="11265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="36">
   <si>
     <t>Start Time</t>
   </si>
@@ -71,9 +72,6 @@
     <t>CT-27</t>
   </si>
   <si>
-    <t>CT-28</t>
-  </si>
-  <si>
     <t>CT-45</t>
   </si>
   <si>
@@ -92,18 +90,12 @@
     <t>CT-66</t>
   </si>
   <si>
-    <t>CT-71</t>
-  </si>
-  <si>
     <t>CT-73</t>
   </si>
   <si>
     <t>CT-74</t>
   </si>
   <si>
-    <t>CT-96</t>
-  </si>
-  <si>
     <t>Connection could not be established</t>
   </si>
   <si>
@@ -132,15 +124,24 @@
   </si>
   <si>
     <t>9/12/2017  14:02:14 PM</t>
+  </si>
+  <si>
+    <t>CT-100</t>
+  </si>
+  <si>
+    <t>CT-44</t>
+  </si>
+  <si>
+    <t>CL-29</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="m/d/yy\ h:mm;@"/>
-    <numFmt numFmtId="168" formatCode="[h]:mm:ss;@"/>
+    <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm;@"/>
+    <numFmt numFmtId="165" formatCode="[h]:mm:ss;@"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -210,8 +211,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -527,24 +528,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:F22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B3:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="13.109375" customWidth="1"/>
-    <col min="3" max="3" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.5546875" customWidth="1"/>
+    <col min="2" max="2" width="13.1796875" customWidth="1"/>
+    <col min="3" max="3" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.54296875" customWidth="1"/>
     <col min="6" max="6" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B3" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>0</v>
@@ -559,113 +560,113 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>13</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>5</v>
@@ -674,160 +675,174 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="5">
+        <v>44540.448611111111</v>
+      </c>
+      <c r="D14" s="5">
+        <v>44540.490277777797</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D18" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F19" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E22" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>